<commit_message>
Added Xenium FOV import.
</commit_message>
<xml_diff>
--- a/datasets/10x_visium_human_brain_cancer.xlsx
+++ b/datasets/10x_visium_human_brain_cancer.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">sample</t>
   </si>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">brain_cancer</t>
   </si>
   <si>
-    <t xml:space="preserve">brain1</t>
+    <t xml:space="preserve">brain</t>
   </si>
   <si>
     <t xml:space="preserve">10x_visium</t>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t xml:space="preserve">ENSEMBL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brain2</t>
   </si>
 </sst>
 </file>
@@ -173,10 +170,10 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.56"/>
   </cols>
@@ -236,29 +233,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>